<commit_message>
safety extra commit before garrett's dumb 1 to 1 way changes
</commit_message>
<xml_diff>
--- a/AutoBlueSystemSrc/customer_product_grid.xlsx
+++ b/AutoBlueSystemSrc/customer_product_grid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\raffettosBlueSystemAddons\AutoBlueSystemSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80D838B-839F-4AA2-A2F3-726C7000FE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87014A8A-BC14-44C1-8ACB-0492A046C72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="5415" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,12 +54,6 @@
     <t>Spinach Linguine</t>
   </si>
   <si>
-    <t>Egg Pappardelle</t>
-  </si>
-  <si>
-    <t>A1PAPP</t>
-  </si>
-  <si>
     <t>A2PAPP</t>
   </si>
   <si>
@@ -70,6 +64,12 @@
   </si>
   <si>
     <t>S1LING</t>
+  </si>
+  <si>
+    <t>Plain Egg Pappardelle</t>
+  </si>
+  <si>
+    <t>01PAPP</t>
   </si>
 </sst>
 </file>
@@ -401,7 +401,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,10 +423,10 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -440,10 +440,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -463,7 +463,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -483,7 +483,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
First commit of Garretts 1 to 1 version.
</commit_message>
<xml_diff>
--- a/AutoBlueSystemSrc/customer_product_grid.xlsx
+++ b/AutoBlueSystemSrc/customer_product_grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\raffettosBlueSystemAddons\AutoBlueSystemSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87014A8A-BC14-44C1-8ACB-0492A046C72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AA564E-CC16-4F3B-9313-04636D6AD2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>gingoso2@gmail.com</t>
   </si>
@@ -42,41 +42,56 @@
     <t>Fettuccine</t>
   </si>
   <si>
-    <t>P1RAVI</t>
-  </si>
-  <si>
-    <t>P1FETT</t>
-  </si>
-  <si>
-    <t>P1LING</t>
-  </si>
-  <si>
     <t>Spinach Linguine</t>
   </si>
   <si>
-    <t>A2PAPP</t>
-  </si>
-  <si>
-    <t>A3PAPP</t>
-  </si>
-  <si>
     <t>Linguine</t>
   </si>
   <si>
-    <t>S1LING</t>
-  </si>
-  <si>
     <t>Plain Egg Pappardelle</t>
   </si>
   <si>
-    <t>01PAPP</t>
+    <t>1 P1RAVI</t>
+  </si>
+  <si>
+    <t>1 P1FETT</t>
+  </si>
+  <si>
+    <t>2 P1FETT</t>
+  </si>
+  <si>
+    <t>1 P1LING</t>
+  </si>
+  <si>
+    <t>1 A2PAPP</t>
+  </si>
+  <si>
+    <t>1 A3PAPP</t>
+  </si>
+  <si>
+    <t>1 case Spinach Fettuccine</t>
+  </si>
+  <si>
+    <t>1 P2FETT</t>
+  </si>
+  <si>
+    <t>2 egg papp</t>
+  </si>
+  <si>
+    <t>1 P1PAPP</t>
+  </si>
+  <si>
+    <t>5 Spinach Linguine</t>
+  </si>
+  <si>
+    <t>5 P2LING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +103,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -398,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +433,7 @@
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -420,76 +441,95 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{17B2EB3B-17CF-4E2D-A4E1-A925EFA4809E}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{749647CF-BA1C-48EA-BEAB-7EE3F77333D8}"/>

</xml_diff>

<commit_message>
Added lbs vs cases. Ready for testing
</commit_message>
<xml_diff>
--- a/AutoBlueSystemSrc/customer_product_grid.xlsx
+++ b/AutoBlueSystemSrc/customer_product_grid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\raffettosBlueSystemAddons\AutoBlueSystemSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AA564E-CC16-4F3B-9313-04636D6AD2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6CE03D-C45E-474F-ACFC-B9C73F623C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>gingoso2@gmail.com</t>
   </si>
@@ -36,55 +36,28 @@
     <t>DONOVON@gmail.com</t>
   </si>
   <si>
-    <t>Ravioli</t>
-  </si>
-  <si>
-    <t>Fettuccine</t>
-  </si>
-  <si>
-    <t>Spinach Linguine</t>
-  </si>
-  <si>
-    <t>Linguine</t>
-  </si>
-  <si>
-    <t>Plain Egg Pappardelle</t>
-  </si>
-  <si>
-    <t>1 P1RAVI</t>
-  </si>
-  <si>
-    <t>1 P1FETT</t>
-  </si>
-  <si>
-    <t>2 P1FETT</t>
-  </si>
-  <si>
-    <t>1 P1LING</t>
-  </si>
-  <si>
-    <t>1 A2PAPP</t>
-  </si>
-  <si>
-    <t>1 A3PAPP</t>
-  </si>
-  <si>
     <t>1 case Spinach Fettuccine</t>
   </si>
   <si>
-    <t>1 P2FETT</t>
-  </si>
-  <si>
     <t>2 egg papp</t>
   </si>
   <si>
-    <t>1 P1PAPP</t>
-  </si>
-  <si>
     <t>5 Spinach Linguine</t>
   </si>
   <si>
-    <t>5 P2LING</t>
+    <t>1 P2FETT cases</t>
+  </si>
+  <si>
+    <t>1 P1PAPP cases</t>
+  </si>
+  <si>
+    <t>5 P2LING cases</t>
+  </si>
+  <si>
+    <t>2 lbs Egg Fettuccine</t>
+  </si>
+  <si>
+    <t>2 P1FETT lbs</t>
   </si>
 </sst>
 </file>
@@ -419,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,99 +406,45 @@
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:10" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
+      <c r="J1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
+      <c r="J2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>